<commit_message>
Added 30 questions geneated using model for Evaluation
</commit_message>
<xml_diff>
--- a/kedronlp/notebooks/Evaluation using Model.xlsx
+++ b/kedronlp/notebooks/Evaluation using Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjan/Bachelor/NLP with Transformers/pubMedNLP/kedronlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A34C9B0-6176-EE49-A44A-4E035F5692F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F95EC9-9D53-B948-9BB3-05B36897A0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>Question Type</t>
   </si>
@@ -190,6 +190,74 @@
   </si>
   <si>
     <t>Since publication in 1982, the 50-item National Adult Reading Test (NART; Nelson, 1982; NART-R; Nelson &amp; Willison, 1991) has remained a widely adopted method for estimating premorbid intelligence both for clinical and research purposes. However, the NART has not been standardised against the most recent revisions of the Wechsler Adult Intelligence Scale (WAIS-III; Wechsler, 1997, and WAIS-IV; Wechsler, 2008). Our objective, therefore, was to produce reliable standardised estimates of WAIS-IV IQ from the NART. Ninety-two neurologically healthy British adults were assessed and regression equations calculated to produce population estimates of WAIS-IV full-scale IQ (FSIQ) and constituent index scores. Results showed strong NART/WAIS-IV FSIQ correlations with more moderate correlations observed between NART error and constituent index scores. FSIQ estimates were closely similar to the published WAIS and WAIS-R estimates at the high end of the distribution, but at the lower end were approximately equidistant from the highly discrepant WAIS (low) and WAIS-R (high) values. We conclude that the NART is likely to remain an important tool for estimating the impact of neurological damage on general cognitive ability. We advise caution in the use of older published WAIS and/or WAIS-R estimates for estimating premorbid WAIS-IV FSIQ, particularly for those with low NART scores.</t>
+  </si>
+  <si>
+    <t>Why</t>
+  </si>
+  <si>
+    <t>Why might the most anterior face patch (AM) show a weaker representation of non-face stimuli than other face patches?</t>
+  </si>
+  <si>
+    <t>Faces are a behaviorally important class of visual stimuli for primates. Recent work in macaque monkeys has identified six discrete face areas where most neurons have higher firing rates to images of faces compared with other objects (Tsao et al., 2006). While neurons in these areas appear to have different tuning (Freiwald and Tsao, 2010; Issa and DiCarlo, 2012), exactly what types of information and, consequently, which visual behaviors neural populations within each face area can support, is unknown. Here we use population decoding to better characterize three of these face patches (ML/MF, AL, and AM). We show that neural activity in all patches contains information that discriminates between the broad categories of face and nonface objects, individual faces, and nonface stimuli. Information is present in both high and lower firing rate regimes. However, there were significant differences between the patches, with the most anterior patch showing relatively weaker representation of nonface stimuli. Additionally, we find that pose-invariant face identity information increases as one moves to more anterior patches, while information about the orientation of the head decreases. Finally, we show that all the information we can extract from the population is present in patterns of activity across neurons, and there is relatively little information in the total activity of the population. These findings give new insight into the representations constructed by the face patch system and how they are successively transformed.</t>
+  </si>
+  <si>
+    <t>How do researchers use population decoding to characterize the neural activity within face patches?</t>
+  </si>
+  <si>
+    <t>Hypothetical</t>
+  </si>
+  <si>
+    <t>If a patient with schizophrenia presents with low IQ and severe negative symptoms, would they be more likely to demonstrate insufficient effort on neuropsychological testing, even if positive symptoms are less pronounced?</t>
+  </si>
+  <si>
+    <t>There is some evidence that insufficient effort may be common in schizophrenia, posing significant threats to the validity of neuropsychological test results. Low effort may account for a significant proportion of variance in neuropsychological test scores and the generalized cognitive deficit that characterizes the disorder. The current study evaluated clinical predictors of insufficient effort in schizophrenia using an embedded effort measure, the Repeatable Battery for the Assessment of Neuropsychological Status (RBANS) Effort Index (EI). Participants were 330 patients meeting DSM-IV-TR criteria for schizophrenia, schizoaffective disorder, or another psychotic disorder who received a battery of neuropsychological tests, including: Wechsler Test of Adult Reading (WTAR), Wechsler Abbreviated Scale of Intelligence (WASI), and RBANS. Clinical assessments designed to measure functional outcome and symptoms were also obtained. Results indicated that 9.4% of patients failed the EI. Patients who failed had lower full-scale, verbal, and performance IQ, as well as poorer performance on RBANS domains not included in the EI (immediate memory, language, and visuospatial/construction). Patients who failed the EI also displayed poorer community-based vocational outcome, greater likelihood of having "deficit schizophrenia" (i.e., primary and enduring negative symptoms), and increased severity of positive symptoms. Regression analyses revealed that insufficient effort was most significantly predicted by a combination of low IQ, negative symptoms, and positive symptoms. Findings suggest that although insufficient effort may be relatively uncommon in schizophrenia, it is associated with important clinical outcomes. The RBANS EI may be a useful tool in evaluating insufficient effort in schizophrenia.</t>
+  </si>
+  <si>
+    <t>If the prevalence of "deficit schizophrenia" increases within a clinical population, might that lead to a corresponding increase in insufficient effort during neuropsychological evaluations?</t>
+  </si>
+  <si>
+    <t>Using a "theory of mind" allows us to explain and predict others' behavior in terms of their mental states, yet individual differences in the accuracy of mental state inferences are not well understood. We hypothesized that the accuracy of mental state inferences can be explained by the ability to characterize the mind giving rise to the mental state. Under this proposal, individuals differentiate between minds by representing them in "Mind-space"-a multidimensional space where dimensions reflect any characteristic of minds that allows them to be individuated. Individual differences in the representation of minds and the accuracy of mental state inferences are explained by one's model of how minds can vary (Mind-space) and ability to locate an individual mind within this space. We measured the accuracy of participants' model of the covariance between dimensions in Mind-space that represent personality traits, and we found this was associated with the accuracy of mental state inference (Experiment 1). Mind-space accuracy also predicted the ability to locate others within Mind-space on dimensions of personality and intelligence (Experiment 2). Direct evidence for the representation of minds in mental state inference was obtained by showing that the location of others in Mind-space affects the probability of particular mental states being ascribed to them (Experiment 3). This latter effect extended to mental states dependent upon representation of trait covariation (Experiment 4). Results support the claim that mental state inference varies according to location in Mind-space, and therefore that adopting the Mind-space framework can explain some of the individual differences in theory of mind. (PsycInfo Database Record (c) 2020 APA, all rights reserved)</t>
+  </si>
+  <si>
+    <t>What factors, besides personality traits and intelligence, might be used as dimensions within an individual's "Mind-space"?</t>
+  </si>
+  <si>
+    <t>Can an individual's "Mind-space" model change or evolve over time?</t>
+  </si>
+  <si>
+    <t>According to the study, which of the following is the primary factor influencing the accuracy of mental state inferences?
+a) The number of dimensions used in an individual's "Mind-space" model
+b) The accuracy of an individual's model of how minds covary
+c) The ability to locate a specific mind within one's "Mind-space"
+d) Pre-existing biases about other people's mental states</t>
+  </si>
+  <si>
+    <t>Intelligent life has emerged late in Earth's habitable lifetime, and required a preceding series of key evolutionary transitions. A simple model (the Carter model) explains the late arrival of intelligent life by positing these evolutionary transitions were exceptionally unlikely 'critical steps'. An alternative model (the neocatastrophism hypothesis) proposes that intelligent life was delayed by frequent catastrophes that served to set back evolutionary innovation. Here, we generalize the Carter model and explore this hypothesis by including catastrophes that can 'undo' an evolutionary transition. Introducing catastrophes or evolutionary dead ends can create situations in which critical steps occur rapidly or in clusters, suggesting that past estimates of the number of critical steps could be underestimated. If catastrophes affect complex life more than simple life, the critical steps will also exhibit a pattern of acceleration towards the present, suggesting that the increase in biological complexity over the past 500 Myr could reflect previously overlooked evolutionary transitions. Furthermore, our results have implications for understanding the different explanations (critical steps versus neo-catastrophes) for the evolution of intelligent life and the so-called Fermi paradox-the observation that intelligent life appears rare in the observable Universe.</t>
+  </si>
+  <si>
+    <t>How does the revised Carter model, which includes catastrophes, change our understanding of the "critical steps" involved in the evolution of intelligent life?</t>
+  </si>
+  <si>
+    <t>Could the apparent increase in biological complexity over the past 500 million years be partially explained by evolutionary transitions that researchers previously hadn't considered?</t>
+  </si>
+  <si>
+    <t>Which hypothesis (critical steps or neo-catastrophes) provides a more plausible explanation for the Fermi paradox?</t>
+  </si>
+  <si>
+    <t>Delay discounting (DD) refers to how rapidly an individual devalues goods based on delays to receipt. DD usually is considered a trait variable but can be state dependent, yet few studies have assessed commodity valuation at short, naturalistically relevant time intervals that might enable state-dependent analysis. This study aimed to determine whether drug-use impulsivity and intelligence influence heroin DD at short (ecologically relevant) delays during two pharmacological states (heroin satiation and withdrawal). Out-of-treatment, intensive heroin users (n = 170; 53.5% African American; 66.7% male) provided complete DD data during imagined heroin satiation and withdrawal. Delays were 3, 6, 12, 24, 48, 72, and 96 hours; maximum delayed heroin amount was thirty $10 bags. Indifference points were used to calculate area under the curve (AUC). We also assessed drug-use impulsivity (subscales from the Impulsive Relapse Questionnaire [IRQ]) and estimated intelligence (Shipley IQ) as predictors of DD. Heroin discounting was greater (smaller AUC) during withdrawal than satiation. In regression analyses, lower intelligence and IRQ Capacity for Delay as well as higher IRQ Speed (to return to drug use) predicted greater heroin discounting in the satiation condition. Lower intelligence and higher IRQ Speed predicted greater discounting in the withdrawal condition. Sex, race, substance use variables, and other IRQ subscales were not significantly related to the withdrawal or satiation DD behavior. In summary, heroin discounting was temporally rapid, pharmacologically state dependent, and predicted by drug-use impulsivity and estimated intelligence. These findings highlight a novel and sensitive measure of acute DD that is easy to administer.</t>
+  </si>
+  <si>
+    <t>Besides drug-use impulsivity and intelligence, what other factors might contribute to differences in heroin delay discounting (DD) during states of satiation and withdrawal?</t>
+  </si>
+  <si>
+    <t>Do the factors predicting heroin DD in a state of satiation differ completely from those predicting DD in a state of withdrawal?</t>
+  </si>
+  <si>
+    <t>Which of the following best summarizes the primary finding of the study?
+a) Heroin delay discounting is not influenced by pharmacological state.
+b) Delay discounting is a trait that remains constant regardless of circumstances.
+c) Heroin delay discounting is influenced by both pharmacological state and individual characteristics.
+d) Intelligence is the single greatest predictor of heroin delay discounting.</t>
   </si>
 </sst>
 </file>
@@ -543,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECB6FD1-CDBE-694D-8700-2DD50D52B540}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,128 +935,245 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Finished 60 questions in Excel file for evaluation
</commit_message>
<xml_diff>
--- a/kedronlp/notebooks/Evaluation using Model.xlsx
+++ b/kedronlp/notebooks/Evaluation using Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjan/Bachelor/NLP with Transformers/pubMedNLP/kedronlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F95EC9-9D53-B948-9BB3-05B36897A0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DAA0E6-5D14-7F4E-915D-1F7E86EB7E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
   <si>
     <t>Question Type</t>
   </si>
@@ -258,6 +258,118 @@
 b) Delay discounting is a trait that remains constant regardless of circumstances.
 c) Heroin delay discounting is influenced by both pharmacological state and individual characteristics.
 d) Intelligence is the single greatest predictor of heroin delay discounting.</t>
+  </si>
+  <si>
+    <t>The continuous development of the society has led to the improvement of people's quality of life and consumption level. At the same time, peoples demand for all aspects of production and life is also increasing, thus promoting the emergence and innovation of intelligent household appliances. To manage these devices conveniently and quickly and enrich family life, "smart home" bureau plays a very important role. Smart home, which enters people's family life, uses communication technology, Internet connection technology, automatic fire control technology, network wiring technology, and visual and audio transmission technology to communicate with home. Mobile terminals have been developed, and more and more PC functions have been realized. Based on the hardware platform of the smart home management system, two solutions were put forward. The first solution is combined with the current 5G network, and through it, the user can control the mobile phone and other mobile terminals on the corresponding application operation instructions to create. The second solution is the design of the web server intelligent management system, for relevant information. It is collected into the database of the server, allows remote access to the node and subscriber information related to storage in the database through the Internet, and searches the information to control the home lighting and temperature. This system is designed to imitate the modular scheme, which includes the central control module, sensor data acquisition module, and software module. Finally, on the browser side and the electronic devices of Android operating system, it realizes the wireless control of lighting, air conditioning, washing machine, and other devices, as well as the detection of the home environment.</t>
+  </si>
+  <si>
+    <t>What specific technologies does the smart home system utilize?</t>
+  </si>
+  <si>
+    <t>Which solution (5G network or web server) offers remote access for controlling home devices?</t>
+  </si>
+  <si>
+    <t>When might a user choose to control their smart home devices from a mobile terminal versus a web interface?</t>
+  </si>
+  <si>
+    <t>Who are the intended users of this smart home system?</t>
+  </si>
+  <si>
+    <t>How does the system enable control of lighting, air conditioning, and other appliances?</t>
+  </si>
+  <si>
+    <t>Target-driven visual navigation is essential for many applications in robotics, and it has gained increasing interest in recent years. In this work, inspired by animal cognitive mechanisms, we propose a novel navigation architecture that simultaneously learns exploration policy and encodes environmental structure. First, to learn exploration policy directly from raw visual input, we use deep reinforcement learning as the basic framework and allow agents to create rewards for themselves as learning signals. In our approach, the reward for the current observation is driven by curiosity and calculated by a count-based approach and temporal distance. While agents learn exploration policy, we use temporal distance to find waypoints in observation sequences and incrementally describe the structure of the environment in a way that integrates episodic memory. Finally, space topological cognition is integrated into the model as a path planning module and combined with a locomotion network to obtain a more generalized approach to navigation. We test our approach in the DMlab, a visually rich 3D environment, and validate its exploration efficiency and navigation performance through extensive experiments. The experimental results show that our approach can explore and encode the environment more efficiently and has better capability in dealing with stochastic objects. In navigation tasks, agents can use space topological cognition to effectively reach the target and guide detour behaviour when a path is unavailable, exhibiting good environmental adaptability.</t>
+  </si>
+  <si>
+    <t>What is the purpose of integrating space topological cognition into the model?</t>
+  </si>
+  <si>
+    <t>Which component of the architecture is responsible for guiding detour behavior?</t>
+  </si>
+  <si>
+    <t>When would an agent rely on space topological cognition instead of direct locomotion for navigation?</t>
+  </si>
+  <si>
+    <t>How do the curiosity-driven rewards influence the agent's exploration behavior?</t>
+  </si>
+  <si>
+    <t>Safety ergonomics is an important branch of safety science and environmental engineering. As humans enter the era of big data, the development of information technology has brought new opportunities and challenges to the innovation, transformation, and upgrading of safety ergonomics, as the traditional safety ergonomics theory has gradually failed to adapt to the need for safe and clean production. Intelligent safety ergonomics (ISE) is regarded as a new direction for the development of safety ergonomics in the era of big data. Unfortunately, since ISE is an emerging concept, there is no research to clarify its basic problems, which leads to a lack of theoretical guidance for the research and practice of ISE. In order to solve the shortcomings of traditional safety ergonomics theories and methods, first of all, this paper answers the basic questions of ISE, including the basic concepts, characteristics, attributes, contents, and research objects. Then, practical application functions of ISE are systematically clarified. Finally, following the life cycle of the design, implementation, operation, and maintenance of the system, it ends with a discussion of the challenges and application prospects of ISE. The conclusion shows that ISE is a cleaner research direction for ergonomics in the era of big data, that it can deepen the understanding of humans, machines, and environment systems, and it can provide a new method for further research on safety and cleaner production. Overall, this paper not only helps safety researchers and practitioners to correctly understand the concept of intelligent safety ergonomics, but it will certainly inject energy and vitality into the development of safety ergonomics and cleaner production.</t>
+  </si>
+  <si>
+    <t>What emerging field of study addresses the limitations of traditional safety ergonomics in the era of big data, aiming to enhance both safety and cleaner production practices?</t>
+  </si>
+  <si>
+    <t>How can the integration of information technology and safety science lead to a more holistic understanding of human-machine-environment systems, ultimately improving workplace safety and sustainability?</t>
+  </si>
+  <si>
+    <t>Many studies have reported attentional biases based on feature-reward associations. However, the effects of location-reward associations on attentional selection remain less well-understood. Unlike feature cases, a previous study that induced participants' awareness of the location-reward association by instructing them to look for a high-reward location has suggested the critical role of goal-driven manipulations in such associations. In this study, we investigated whether the reward effect occurred without goal-driven manipulations if participants were spontaneously aware of the location-reward association. We conducted three experiments using a visual search task that included four circles where participants received rewards; one possible target location was associated with a high reward, and another with a low reward. In Experiment 1, the target was presented among distractors, and participants had to search for the target. The results showed a faster reaction time in the high-reward rather than the low-reward locations only in participants aware of the location-reward association, even if they were not required to look for the association. Moreover, in Experiment 2, we replicated the main findings of Experiment 1, even when the target had an abrupt visual onset to restrict goal-driven manipulations. Furthermore, Experiment 3 confirmed that the effect observed in Experiment 2 could not be attributed to the initial eye position. These findings suggest that goal-driven manipulations are unnecessary for inducing reward biases to high-reward locations. We concluded that awareness of the association rather than goal-driven manipulations is crucial for the location-reward effect.</t>
+  </si>
+  <si>
+    <t>How does the study challenge previous findings about the role of goal-driven manipulation in location-reward association?</t>
+  </si>
+  <si>
+    <t>Did the researchers find a significant location-reward effect even when participants were not actively searching for high-reward locations?</t>
+  </si>
+  <si>
+    <t>Which factor appears to be the most important for inducing a reward bias in the study?
+a) Presence of a reward
+b) Awareness of location-reward association
+c) Goal-driven search for high-reward locations
+d) Abrupt onset of the target</t>
+  </si>
+  <si>
+    <t>Background: A Primary Care Model Programme was implemented in Hungary between 2013 and 2017 in order to increase access of disadvantaged population groups to primary care and to offer new preventive services for all clients. In a country with single-handed practices, four group practices or GP clusters were created in the Programme. Six GPs comprised one cluster who together employed nonmedical health professionals and nonprofessional health mediators, the latter recruited from the serviced communities, many of them of Roma ethnicity. Health mediators were tasked by improving access of the local communities - including its vulnerable Roma members - to existing and new services. Health mediators were interviewed about their work experiences, motivation, and overall opinion as members of the clusters as part of the Programme evaluation.
+Methods: As part of the Programme evaluation, structured interviews were conducted with all 40 health mediators employed at the time in the Programme. Interviews were transcribed and content analysis was carried out.
+Results: Three themes emerged from the transcripts. The first focused on the health mediators' personal characteristics such as motivation to join the Programme, the way their job increased their self-esteem, social status and health consciousness. Domains of the second theme of their work included importance of on-the-job training and of their insider knowledge of local communities, as well as their pride to have become members of the primary care team. The third theme covered overall functioning of the Programme of which they had mostly positive opinions, notwithstanding some criticism regarding procurement.
+Conclusions: Health mediators had earlier worked in various European countries specifically to improve access of Roma ethnic groups to health services but the Hungarian Model Programme was globally the first in which health mediators as non-professional workers became equal members of the primary care team as employees. Their contribution and overwhelmingly positive experiences, along with their useful insights for improvement call for the establishment and funding of health mediator positions in primary care especially in areas with large numbers of disadvantaged Roma populations.</t>
+  </si>
+  <si>
+    <t>What were the primary goals of the Hungarian Primary Care Model Programme?</t>
+  </si>
+  <si>
+    <t>Who were the primary beneficiaries of the health mediator's work?</t>
+  </si>
+  <si>
+    <t>How did the health mediators' work increase their self-esteem and social status?</t>
+  </si>
+  <si>
+    <t>Why is the use of health mediators particularly important in areas with disadvantaged Roma populations?</t>
+  </si>
+  <si>
+    <t>Where were the GP clusters implementing the Primary Care Model Programme located?</t>
+  </si>
+  <si>
+    <t>Where</t>
+  </si>
+  <si>
+    <t>When did the evaluation of the Primary Care Model Programme take place?</t>
+  </si>
+  <si>
+    <t>Which of the health mediators' job aspects received the most positive feedback?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How can clinicians improve their communication with patients to cultivate stronger relationships and promote better adherence to dietary recommendations? </t>
+  </si>
+  <si>
+    <t>Why is it crucial for clinicians to recognize their own implicit biases about weight and food?</t>
+  </si>
+  <si>
+    <t>For clinicians, effective communication goes beyond the delivery of scientific information to include an understanding of who the patient is and what they value; treating them with respect; and acknowledging their emotional and social realities. Recognizing our own implicit biases and cultivating a more mindful approach to the impact of language, especially around weight and food, and using verbal and nonverbal approaches to convey empathic concern can improve our relationships with our patients. Patients who feel seen and respected are more likely to follow through with recommendations including dietary change, leading to improved health and quality of life.</t>
+  </si>
+  <si>
+    <t>How does a leader's level of trait empathy influence their emotional reactions and perceived effectiveness after providing negative feedback?</t>
+  </si>
+  <si>
+    <t>Although providing negative performance feedback can enhance employee performance, leaders are sometimes reluctant to engage in this activity. Reflecting this, prior research has identified negative feedback provision as an aversive, yet potentially rewarding, managerial activity. However, little is known about how providing negative feedback impacts the effectiveness of leaders who do so. To shed light on this issue, we develop and test a theoretical model that identifies how leaders' proximal and distal reactions to providing negative feedback are contingent upon their levels of trait empathy. Supporting our theory, results from an experience sampling study indicate that leaders higher in trait empathy report feeling both less attentive and more distressed after providing subordinates with negative feedback, whereas leaders lower in trait empathy report feeling more attentive and less distressed. Attentiveness and distress, in turn, were associated with leaders' daily perceptions of their effectiveness; distress was also associated with leaders' daily enactment of transformational leadership behavior. Results of two subsequent studies focused on single episodes of negative feedback provision revealed that trait empathy amplifies the extent to which feedback recipients' negative emotional reactions impact additional leader effectiveness criteria (e.g., executive functioning and planning/problem-solving), further supporting the need to account for the crucial role of trait empathy in the feedback-provision process. Altogether, our research provides a novel perspective on the feedback-giving process by shifting the focus of theorizing from the recipient to the provider, while challenging current thinking about leader empathy by highlighting its potential downside for leadership. (PsycInfo Database Record (c) 2022 APA, all rights reserved).</t>
+  </si>
+  <si>
+    <t>Does the study suggest that there are potential downsides to leader empathy in the context of giving negative feedback?</t>
+  </si>
+  <si>
+    <t>How can nurse leaders use emotional intelligence to specifically address the challenges of stress, exhaustion, and the risk of moral injury brought on by the COVID-19 pandemic?</t>
+  </si>
+  <si>
+    <t>Emotionally intelligent leaders demonstrate a sensitivity to their own and other people's psychological health and well-being, directing others towards common goals while developing effective personal relationships with their colleagues and team members. Emotional intelligence is particularly relevant in the context of the coronavirus disease 2019 pandemic, where nurse leaders need to demonstrate this skill when supporting their teams to manage high levels of stress, exhaustion and the risk of moral injury. This article explores emotional intelligence, discusses its importance as a characteristic of effective nurse leaders and managers, and suggests practical activities that leaders can undertake to develop their emotional intelligence skills.</t>
   </si>
 </sst>
 </file>
@@ -611,9 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECB6FD1-CDBE-694D-8700-2DD50D52B540}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1076,7 +1186,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
@@ -1117,130 +1227,364 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shifted abstracts to be context and added shorter ChatGPT generated answers for all 60 questions in Excel file
</commit_message>
<xml_diff>
--- a/kedronlp/notebooks/Evaluation using Model.xlsx
+++ b/kedronlp/notebooks/Evaluation using Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjan/Bachelor/NLP with Transformers/pubMedNLP/kedronlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93F2A95-ED92-FF48-A39B-972F4E4C8911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30E995E-341F-EB4B-9270-E6AED728764C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{3AC1803B-D431-F74E-BDCB-3D80AD30DE94}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="160">
   <si>
     <t>Question Type</t>
   </si>
@@ -367,6 +367,190 @@
   </si>
   <si>
     <t>Emotionally intelligent leaders demonstrate a sensitivity to their own and other people's psychological health and well-being, directing others towards common goals while developing effective personal relationships with their colleagues and team members. Emotional intelligence is particularly relevant in the context of the coronavirus disease 2019 pandemic, where nurse leaders need to demonstrate this skill when supporting their teams to manage high levels of stress, exhaustion and the risk of moral injury. This article explores emotional intelligence, discusses its importance as a characteristic of effective nurse leaders and managers, and suggests practical activities that leaders can undertake to develop their emotional intelligence skills.</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>There might be no significant differences in conscientious intelligence sub-dimensions between first and fourth-year nursing students because the study found that factors such as willingness to choose nursing as a profession, gender (female), and not perceiving nursing as solely a means to earn money were more influential in determining conscientious intelligence scores than academic year level.</t>
+  </si>
+  <si>
+    <t>Yes, according to the study, nursing students who do not perceive nursing as solely a means to earn money demonstrate higher levels of conscientious intelligence.</t>
+  </si>
+  <si>
+    <t>b) Willingness to choose the profession</t>
+  </si>
+  <si>
+    <t>The study quantitatively demonstrates the relationship between IQ and brain resilience by utilizing resting-state fMRI graph-theoretical analysis in 102 healthy individuals. They observe enhanced brain robustness to targeted attacks (TA) in individuals with higher IQ, indicating increased distributed processing capacity despite the systematic loss of important nodes. Additionally, they identify specific neocortical regions, primarily involved in language and memory processing networks, associated with brain resilience in higher IQ individuals, while emotional processing regions are more relevant for lower IQ individuals.</t>
+  </si>
+  <si>
+    <t>Yes, individuals with higher IQ show resilience to both targeted and random attacks on the brain, as evidenced by the study's findings. The enhanced brain robustness to targeted attacks (TA) in individuals with higher IQ indicates increased distributed processing capacity despite the systematic loss of important nodes. Additionally, brain resilience in higher IQ individuals is supported by a set of neocortical regions mainly involved in language and memory processing networks.</t>
+  </si>
+  <si>
+    <t>a) Higher IQ: Neocortical regions mainly belonging to language and memory processing networks.
+b) Lower IQ: Regions related to emotional processing.</t>
+  </si>
+  <si>
+    <t>Exposure to lead-based industries can negatively impact the intelligence of school-aged children by interfering with brain development and function, leading to cognitive impairments, as evidenced by a negative correlation between blood lead levels and intelligence scores.</t>
+  </si>
+  <si>
+    <t>Nutritional supplementation and hygiene education had a greater impact on reducing lead levels in the experimental group compared to improving intelligence scores.</t>
+  </si>
+  <si>
+    <t>c) Lead exposure may not directly impact hemoglobin levels.</t>
+  </si>
+  <si>
+    <t>The study provides evidence supporting the use of new tools for measuring mindsets in medical education through the satisfactory psychometric properties demonstrated by the new items. Additionally, the study's findings reveal the impact of mindsets on medical education, suggesting the potential usefulness of these tools in understanding and assessing clinical supervisors' beliefs about the fixed versus learnable nature of attributes such as intelligence, clinical reasoning, moral character, and empathy.</t>
+  </si>
+  <si>
+    <t>The greatest percentage of clinical supervisors viewed empathy as fixed.</t>
+  </si>
+  <si>
+    <t>A clinical supervisor's mindset about a particular attribute might impact their teaching practices when they believe that attribute to be fixed rather than learnable. For example, if a supervisor believes that empathy is fixed and cannot be developed through education and training, they may be less likely to emphasize or prioritize empathy-related skills in their teaching. This could result in a teaching approach that focuses less on cultivating empathy in medical students or residents, potentially affecting the quality of patient care and interpersonal interactions.</t>
+  </si>
+  <si>
+    <t>Medical educators, curriculum developers, and policymakers might benefit from better understanding the impact of mindsets on medical education.</t>
+  </si>
+  <si>
+    <t>The researchers measured the clinical supervisors' mindsets using surveys containing existing instruments for intelligence and moral character, as well as 18 new items for assessing clinical reasoning and empathy.</t>
+  </si>
+  <si>
+    <t>The PCTB assesses areas of cognition including physical cognition (e.g., quantity discrimination) and social cognition (e.g., gaze following) in chimpanzees.</t>
+  </si>
+  <si>
+    <t>The factor in the PCTB most strongly related to HDT efficiency was chimpanzee g scores.</t>
+  </si>
+  <si>
+    <t>A chimpanzee's self-control abilities might be most critical for successful performance on the PCTB when they need to sustain delay of gratification while engaging in tasks that require cognitive processing, such as quantity discrimination or gaze following.</t>
+  </si>
+  <si>
+    <t>Besides chimpanzees, humans also demonstrate a link between general intelligence and self-control behavior.</t>
+  </si>
+  <si>
+    <t>The Hybrid Delay Task (HDT) measures self-control in chimpanzees by assessing their inter-temporal choices and capacity for sustained delay of gratification.</t>
+  </si>
+  <si>
+    <t>The NART-derived WAIS-IV FSIQ estimates are approximately equidistant from the highly discrepant WAIS (low) and WAIS-R (high) values, particularly at the lower end of the distribution.</t>
+  </si>
+  <si>
+    <t>The pattern of correlations between NART performance and the different WAIS-IV measures showed strong correlations with WAIS-IV Full-Scale IQ (FSIQ) and more moderate correlations with constituent index scores. There were differences in the strength of correlations across the board, with FSIQ showing stronger correlations compared to constituent index scores. Additionally, correlations with NART error scores were more moderate compared to correlations with FSIQ.</t>
+  </si>
+  <si>
+    <t>The most anterior face patch (AM) might show a weaker representation of non-face stimuli compared to other face patches because it likely specializes more in processing facial information rather than non-face visual stimuli.</t>
+  </si>
+  <si>
+    <t>Researchers use population decoding to characterize the neural activity within face patches by analyzing patterns of activity across neurons to decode information related to discriminating between face and nonface objects, individual faces, and nonface stimuli.</t>
+  </si>
+  <si>
+    <t>Yes, according to the study, patients with schizophrenia who have low IQ and severe negative symptoms are more likely to demonstrate insufficient effort on neuropsychological testing, even if positive symptoms are less pronounced.</t>
+  </si>
+  <si>
+    <t>Yes, according to the study, an increased prevalence of "deficit schizophrenia" within a clinical population might lead to a corresponding increase in insufficient effort during neuropsychological evaluations.</t>
+  </si>
+  <si>
+    <t>Besides personality traits and intelligence, other factors that might be used as dimensions within an individual's "Mind-space" could include beliefs, emotions, values, attitudes, preferences, and social roles.</t>
+  </si>
+  <si>
+    <t>Yes, an individual's "Mind-space" model can change or evolve over time as they gain new experiences, encounter different social situations, and acquire new knowledge about the variability of mental states and personality traits.</t>
+  </si>
+  <si>
+    <t>b) The accuracy of an individual's model of how minds covary</t>
+  </si>
+  <si>
+    <t>The revised Carter model, incorporating catastrophes, suggests that past estimates of critical steps in the evolution of intelligent life may have been underestimated. It proposes that catastrophes can accelerate or cluster critical steps, potentially leading to a more rapid emergence of intelligent life.</t>
+  </si>
+  <si>
+    <t>Yes, the apparent increase in biological complexity over the past 500 million years could be partially explained by previously overlooked evolutionary transitions, including those influenced by catastrophes, according to the generalized Carter model.</t>
+  </si>
+  <si>
+    <t>The neo-catastrophes hypothesis provides a more plausible explanation for the Fermi paradox, which observes the rarity of intelligent life in the observable Universe.</t>
+  </si>
+  <si>
+    <t>Besides drug-use impulsivity and intelligence, other factors that might contribute to differences in heroin delay discounting (DD) during states of satiation and withdrawal could include individual differences in physiological arousal, emotional state, or cognitive functioning specific to each state. Additionally, environmental factors, such as the presence of cues associated with drug use or stressors, could also influence DD during these states.</t>
+  </si>
+  <si>
+    <t>No, the factors predicting heroin delay discounting (DD) in a state of satiation partially overlap with those predicting DD in a state of withdrawal. Lower intelligence and higher IRQ Speed (to return to drug use) predicted greater discounting in both states, while lower IRQ Capacity for Delay predicted greater discounting only in the satiation condition.</t>
+  </si>
+  <si>
+    <t>c) Heroin delay discounting is influenced by both pharmacological state and individual characteristics.</t>
+  </si>
+  <si>
+    <t>The smart home system utilizes communication technology, Internet connection technology, automatic fire control technology, network wiring technology, and visual and audio transmission technology.</t>
+  </si>
+  <si>
+    <t>The web server intelligent management system offers remote access for controlling home devices.</t>
+  </si>
+  <si>
+    <t>A user might choose to control their smart home devices from a mobile terminal when they are on the go or prefer a more portable option. They might opt for a web interface when they are at a stationary location with access to a computer or prefer a larger screen for control.</t>
+  </si>
+  <si>
+    <t>The intended users of this smart home system are homeowners or individuals looking to manage and control household appliances and systems for convenience and efficiency.</t>
+  </si>
+  <si>
+    <t>The system enables control of lighting, air conditioning, and other appliances wirelessly through mobile terminals or web interfaces connected to the smart home management system.</t>
+  </si>
+  <si>
+    <t>The purpose of integrating space topological cognition into the model is to serve as a path planning module, enabling the model to obtain a more generalized approach to navigation.</t>
+  </si>
+  <si>
+    <t>The space topological cognition component is responsible for guiding detour behavior in the navigation architecture.</t>
+  </si>
+  <si>
+    <t>An agent would rely on space topological cognition instead of direct locomotion for navigation when a path to the target is unavailable, requiring detour behavior.</t>
+  </si>
+  <si>
+    <t>The curiosity-driven rewards influence the agent's exploration behavior by incentivizing it to explore novel and uncertain regions of the environment, leading to more comprehensive exploration and learning.</t>
+  </si>
+  <si>
+    <t>The emerging field of study addressing the limitations of traditional safety ergonomics in the era of big data is called Intelligent Safety Ergonomics (ISE).</t>
+  </si>
+  <si>
+    <t>The integration of information technology and safety science, as seen in Intelligent Safety Ergonomics (ISE), can lead to a more holistic understanding of human-machine-environment systems by providing deeper insights into their interactions and dynamics. This understanding can lead to improved workplace safety and sustainability through more informed decision-making and the development of innovative solutions tailored to specific contexts and challenges.</t>
+  </si>
+  <si>
+    <t>The study challenges previous findings by demonstrating that awareness of the location-reward association, rather than goal-driven manipulations, is crucial for inducing reward biases to high-reward locations.</t>
+  </si>
+  <si>
+    <t>Yes, the researchers found a significant location-reward effect even when participants were not actively searching for high-reward locations.</t>
+  </si>
+  <si>
+    <t>b) Awareness of location-reward association</t>
+  </si>
+  <si>
+    <t>The primary goals of the Hungarian Primary Care Model Programme were to increase access to primary care for disadvantaged population groups and to offer new preventive services for all clients.</t>
+  </si>
+  <si>
+    <t>The primary beneficiaries of the health mediator's work were the local communities, including vulnerable Roma members, who aimed to improve access to health services.</t>
+  </si>
+  <si>
+    <t>The health mediators' work increased their self-esteem and social status by allowing them to become equal members of the primary care team, contributing to the improvement of access to health services for disadvantaged populations.</t>
+  </si>
+  <si>
+    <t>The use of health mediators is particularly important in areas with disadvantaged Roma populations because they can improve access to health services for this vulnerable group, addressing their specific needs and increasing their utilization of preventive and primary care.</t>
+  </si>
+  <si>
+    <t>The GP clusters implementing the Primary Care Model Programme were located in Hungary.</t>
+  </si>
+  <si>
+    <t>The evaluation of the Primary Care Model Programme took place between 2013 and 2017 in Hungary.</t>
+  </si>
+  <si>
+    <t>The health mediators' job aspects related to their personal characteristics, such as motivation, increased self-esteem, social status, and health consciousness, received the most positive feedback.</t>
+  </si>
+  <si>
+    <t>Clinicians can improve their communication by understanding patients' values, treating them with respect, acknowledging emotional and social realities, recognizing implicit biases, being mindful of language around weight and food, and using verbal and nonverbal approaches to convey empathic concern.</t>
+  </si>
+  <si>
+    <t>It's crucial for clinicians to recognize their own implicit biases about weight and food to ensure they communicate with patients in a respectful and nonjudgmental manner, fostering stronger relationships and promoting better adherence to dietary recommendations.</t>
+  </si>
+  <si>
+    <t>A leader's level of trait empathy influences their emotional reactions and perceived effectiveness after providing negative feedback. Leaders higher in trait empathy report feeling less attentive and more distressed, while those lower in trait empathy feel more attentive and less distressed.</t>
+  </si>
+  <si>
+    <t>Yes, the study suggests that there are potential downsides to leader empathy in the context of giving negative feedback.</t>
+  </si>
+  <si>
+    <t>Nurse leaders can use emotional intelligence to specifically address the challenges of stress, exhaustion, and the risk of moral injury brought on by the COVID-19 pandemic by supporting their teams, fostering effective personal relationships, and directing them towards common goals while demonstrating sensitivity to their psychological health and well-being.</t>
   </si>
 </sst>
 </file>
@@ -718,7 +902,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECB6FD1-CDBE-694D-8700-2DD50D52B540}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -729,7 +913,7 @@
     <col min="3" max="3" width="46.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -737,10 +921,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -750,8 +937,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -761,8 +951,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -772,8 +965,11 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -783,8 +979,11 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -794,8 +993,11 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -805,8 +1007,11 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -816,8 +1021,11 @@
       <c r="C8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -827,8 +1035,11 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -838,8 +1049,11 @@
       <c r="C10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -849,8 +1063,11 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -860,8 +1077,11 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -871,8 +1091,11 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -882,8 +1105,11 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -893,8 +1119,11 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -904,8 +1133,11 @@
       <c r="C16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -915,8 +1147,11 @@
       <c r="C17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -926,8 +1161,11 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -937,8 +1175,11 @@
       <c r="C19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -948,8 +1189,11 @@
       <c r="C20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -959,8 +1203,11 @@
       <c r="C21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -970,8 +1217,11 @@
       <c r="C22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -981,8 +1231,11 @@
       <c r="C23" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -992,8 +1245,11 @@
       <c r="C24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1003,8 +1259,11 @@
       <c r="C25" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1014,8 +1273,11 @@
       <c r="C26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1025,8 +1287,11 @@
       <c r="C27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1036,8 +1301,11 @@
       <c r="C28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1047,8 +1315,11 @@
       <c r="C29" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -1058,8 +1329,11 @@
       <c r="C30" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1069,8 +1343,11 @@
       <c r="C31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1080,8 +1357,11 @@
       <c r="C32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1091,8 +1371,11 @@
       <c r="C33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1102,8 +1385,11 @@
       <c r="C34" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1113,8 +1399,11 @@
       <c r="C35" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -1124,8 +1413,11 @@
       <c r="C36" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1135,8 +1427,11 @@
       <c r="C37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -1146,8 +1441,11 @@
       <c r="C38" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -1157,8 +1455,11 @@
       <c r="C39" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1168,8 +1469,11 @@
       <c r="C40" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -1179,8 +1483,11 @@
       <c r="C41" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -1190,8 +1497,11 @@
       <c r="C42" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -1201,8 +1511,11 @@
       <c r="C43" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1212,8 +1525,11 @@
       <c r="C44" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1223,8 +1539,11 @@
       <c r="C45" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -1234,8 +1553,11 @@
       <c r="C46" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1245,8 +1567,11 @@
       <c r="C47" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1256,8 +1581,11 @@
       <c r="C48" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1267,8 +1595,11 @@
       <c r="C49" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -1278,8 +1609,11 @@
       <c r="C50" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -1289,8 +1623,11 @@
       <c r="C51" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -1300,8 +1637,11 @@
       <c r="C52" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -1311,8 +1651,11 @@
       <c r="C53" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -1322,8 +1665,11 @@
       <c r="C54" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>27</v>
       </c>
@@ -1333,8 +1679,11 @@
       <c r="C55" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -1344,8 +1693,11 @@
       <c r="C56" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -1355,8 +1707,11 @@
       <c r="C57" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>44</v>
       </c>
@@ -1366,8 +1721,11 @@
       <c r="C58" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -1377,8 +1735,11 @@
       <c r="C59" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -1388,8 +1749,11 @@
       <c r="C60" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -1398,6 +1762,9 @@
       </c>
       <c r="C61" t="s">
         <v>98</v>
+      </c>
+      <c r="D61" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>